<commit_message>
Updated the info section to now have delve
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/twisted-memories-delve-monsters.xlsx
+++ b/resources/data-imports/Monsters/twisted-memories-delve-monsters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">795381477075-997181360106</t>
   </si>
   <si>
-    <t xml:space="preserve">Purgatory</t>
+    <t xml:space="preserve">Twisted Memories</t>
   </si>
   <si>
     <t xml:space="preserve">Corrupted Spirit of Torment</t>
@@ -199,9 +199,6 @@
     <t xml:space="preserve">868653926499-1072383125762</t>
   </si>
   <si>
-    <t xml:space="preserve">Vile of Innocence</t>
-  </si>
-  <si>
     <t xml:space="preserve">Forgotten Memories of Pain</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t xml:space="preserve">948676409711-1153256182302</t>
   </si>
   <si>
-    <t xml:space="preserve">Flask of ever lasting water</t>
-  </si>
-  <si>
     <t xml:space="preserve">Magician of Lies</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
     <t xml:space="preserve">1066956025251-1270652761049</t>
   </si>
   <si>
-    <t xml:space="preserve">Wild Game Meat</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fiend of the Depths</t>
   </si>
   <si>
@@ -272,9 +263,6 @@
   </si>
   <si>
     <t xml:space="preserve">1199982573790-1399999812651</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flame of the Prince</t>
   </si>
 </sst>
 </file>
@@ -585,8 +573,8 @@
   </sheetPr>
   <dimension ref="A1:AX16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AX2" activeCellId="0" sqref="AX2:AX16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM11" activeCellId="0" sqref="AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1260,11 +1248,8 @@
       <c r="AL5" s="1" t="n">
         <v>0.336991670880446</v>
       </c>
-      <c r="AM5" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="AN5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>52</v>
@@ -1278,7 +1263,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>780772601324.805</v>
@@ -1344,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA6" s="3" t="n">
         <v>780772601324.805</v>
@@ -1400,7 +1385,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>827722722083.01</v>
@@ -1466,10 +1451,10 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA7" s="3" t="n">
         <v>827722722083.01</v>
@@ -1522,7 +1507,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>877496089757.755</v>
@@ -1588,10 +1573,10 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA8" s="3" t="n">
         <v>877496089757.755</v>
@@ -1629,11 +1614,8 @@
       <c r="AL8" s="1" t="n">
         <v>0.403112868146337</v>
       </c>
-      <c r="AM8" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="AN8" s="1" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AO8" s="1" t="s">
         <v>52</v>
@@ -1647,7 +1629,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>930262474373.549</v>
@@ -1713,10 +1695,10 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AA9" s="3" t="n">
         <v>930262474373.549</v>
@@ -1769,7 +1751,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>986201854718.806</v>
@@ -1835,10 +1817,10 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA10" s="3" t="n">
         <v>986201854718.806</v>
@@ -1891,7 +1873,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>1045505032228.43</v>
@@ -1957,10 +1939,10 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AA11" s="3" t="n">
         <v>1045505032228.43</v>
@@ -2013,7 +1995,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>1108374281780.92</v>
@@ -2079,10 +2061,10 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AA12" s="3" t="n">
         <v>1108374281780.92</v>
@@ -2120,11 +2102,8 @@
       <c r="AL12" s="1" t="n">
         <v>0.511882153670112</v>
       </c>
-      <c r="AM12" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="AN12" s="1" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="AO12" s="1" t="s">
         <v>52</v>
@@ -2138,7 +2117,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>1175024041629.82</v>
@@ -2204,10 +2183,10 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AA13" s="3" t="n">
         <v>1175024041629.82</v>
@@ -2260,7 +2239,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>1245681644822.74</v>
@@ -2326,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AA14" s="3" t="n">
         <v>1245681644822.74</v>
@@ -2382,7 +2361,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>1320588094602.7</v>
@@ -2448,10 +2427,10 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="AA15" s="3" t="n">
         <v>1320588094602.7</v>
@@ -2504,7 +2483,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>1399998886436.64</v>
@@ -2570,10 +2549,10 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AA16" s="3" t="n">
         <v>1399998886436.64</v>
@@ -2611,11 +2590,9 @@
       <c r="AL16" s="1" t="n">
         <v>0.649999937860663</v>
       </c>
-      <c r="AM16" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="AM16" s="5"/>
       <c r="AN16" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO16" s="1" t="s">
         <v>52</v>

</xml_diff>